<commit_message>
Retailer Updates (in progress)
</commit_message>
<xml_diff>
--- a/Overview - Retailers.xlsx
+++ b/Overview - Retailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4FB7B0-E3BD-414A-9530-57BB25DFB5FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4F32D8-DC42-4C9E-97D6-369583C47489}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25680" windowHeight="10815" xr2:uid="{8CE0BD80-0294-417F-B513-C2C882DCE57C}"/>
   </bookViews>
@@ -201,7 +201,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0\x"/>
+    <numFmt numFmtId="164" formatCode="0.0\x"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -287,7 +287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -322,9 +322,6 @@
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -337,10 +334,22 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -502,6 +511,9 @@
           <cell r="V28">
             <v>0.1075657234597632</v>
           </cell>
+          <cell r="AH28">
+            <v>0.08</v>
+          </cell>
         </row>
         <row r="29">
           <cell r="V29">
@@ -511,6 +523,16 @@
         <row r="30">
           <cell r="V30">
             <v>0.20183486238532111</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="AH32">
+            <v>9.7255299689414816</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="AH34">
+            <v>0.69584996581308856</v>
           </cell>
         </row>
       </sheetData>
@@ -604,33 +626,33 @@
       </sheetData>
       <sheetData sheetId="1">
         <row r="16">
-          <cell r="V16">
+          <cell r="X16">
             <v>1.4491480765852716E-2</v>
           </cell>
-          <cell r="W16">
+          <cell r="Y16">
             <v>0.11877759501341889</v>
           </cell>
-          <cell r="X16">
+          <cell r="Z16">
             <v>5.9815832237096522E-2</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="X19">
+          <cell r="Z19">
             <v>0.52694217289719625</v>
           </cell>
         </row>
         <row r="20">
-          <cell r="X20">
+          <cell r="Z20">
             <v>7.878212616822429E-2</v>
           </cell>
         </row>
         <row r="21">
-          <cell r="X21">
+          <cell r="Z21">
             <v>5.6731892523364483E-2</v>
           </cell>
         </row>
         <row r="22">
-          <cell r="X22">
+          <cell r="Z22">
             <v>0.19565217391304351</v>
           </cell>
         </row>
@@ -940,10 +962,10 @@
   <dimension ref="B1:AX8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AB3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AL8" sqref="AL8"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -955,7 +977,8 @@
     <col min="6" max="6" width="9.140625" style="10"/>
     <col min="7" max="10" width="9.140625" style="11"/>
     <col min="11" max="12" width="9.140625" style="2"/>
-    <col min="13" max="15" width="9.140625" style="3"/>
+    <col min="13" max="13" width="9.140625" style="20"/>
+    <col min="14" max="15" width="9.140625" style="3"/>
     <col min="16" max="16" width="9.140625" style="1"/>
     <col min="17" max="21" width="9.140625" style="2"/>
     <col min="22" max="22" width="9.140625" style="1"/>
@@ -975,31 +998,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:50" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="W1" s="14" t="s">
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="W1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="23"/>
       <c r="AC1" s="2"/>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="15"/>
-      <c r="AL1" s="15"/>
-      <c r="AM1" s="15"/>
-      <c r="AN1" s="15"/>
-      <c r="AO1" s="15"/>
-      <c r="AP1" s="15"/>
-      <c r="AR1" s="16"/>
+      <c r="AI1" s="14"/>
+      <c r="AJ1" s="14"/>
+      <c r="AK1" s="14"/>
+      <c r="AL1" s="14"/>
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="14"/>
+      <c r="AO1" s="14"/>
+      <c r="AP1" s="14"/>
+      <c r="AR1" s="15"/>
     </row>
     <row r="2" spans="2:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
@@ -1035,7 +1058,7 @@
       <c r="L2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="21" t="s">
         <v>11</v>
       </c>
       <c r="N2" s="5" t="s">
@@ -1090,31 +1113,31 @@
       <c r="AG2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AI2" s="17" t="s">
+      <c r="AI2" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="AJ2" s="17" t="s">
+      <c r="AJ2" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AK2" s="17" t="s">
+      <c r="AK2" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="AL2" s="17" t="s">
+      <c r="AL2" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="AM2" s="17" t="s">
+      <c r="AM2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="AN2" s="17" t="s">
+      <c r="AN2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="AO2" s="17" t="s">
+      <c r="AO2" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="AP2" s="17" t="s">
+      <c r="AP2" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="AR2" s="18" t="s">
+      <c r="AR2" s="17" t="s">
         <v>39</v>
       </c>
       <c r="AS2" s="7" t="s">
@@ -1174,99 +1197,111 @@
         <f>[1]Main!$D$31</f>
         <v>45096</v>
       </c>
-      <c r="Q4" s="19">
+      <c r="M4" s="20">
+        <f>'[1]Financial Model'!$AH$32</f>
+        <v>9.7255299689414816</v>
+      </c>
+      <c r="N4" s="22">
+        <f>'[1]Financial Model'!$AH$34</f>
+        <v>0.69584996581308856</v>
+      </c>
+      <c r="O4" s="22">
+        <f>'[1]Financial Model'!$AH$28</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q4" s="18">
         <f>[1]Main!$C$36</f>
         <v>7.9778273551388885</v>
       </c>
-      <c r="R4" s="19">
+      <c r="R4" s="18">
         <f>[1]Main!$C$37</f>
         <v>1.152726408930363</v>
       </c>
-      <c r="S4" s="19">
+      <c r="S4" s="18">
         <f>[1]Main!$C$38</f>
         <v>1.2964149499698976</v>
       </c>
-      <c r="T4" s="19">
+      <c r="T4" s="18">
         <f>[1]Main!$C$39</f>
         <v>14.880921491450774</v>
       </c>
-      <c r="U4" s="19">
+      <c r="U4" s="18">
         <f>[1]Main!$C$40</f>
         <v>18.563320964655169</v>
       </c>
-      <c r="W4" s="16">
+      <c r="W4" s="15">
         <f>'[1]Financial Model'!$V$16</f>
         <v>348</v>
       </c>
-      <c r="X4" s="16">
+      <c r="X4" s="15">
         <f>'[1]Financial Model'!$U$16</f>
         <v>422</v>
       </c>
-      <c r="Y4" s="16">
+      <c r="Y4" s="15">
         <f>'[1]Financial Model'!$T$16</f>
         <v>428.10400000000021</v>
       </c>
-      <c r="Z4" s="16">
+      <c r="Z4" s="15">
         <f>'[1]Financial Model'!$S$16</f>
         <v>194.77700000000002</v>
       </c>
-      <c r="AA4" s="16">
+      <c r="AA4" s="15">
         <f>'[1]Financial Model'!$R$16</f>
         <v>202.15100000000001</v>
       </c>
-      <c r="AB4" s="16">
+      <c r="AB4" s="15">
         <f>'[1]Financial Model'!$Q$16</f>
         <v>185.44100000000026</v>
       </c>
-      <c r="AD4" s="15">
+      <c r="AD4" s="14">
         <f>'[1]Financial Model'!$V$27</f>
         <v>0.36142885811759984</v>
       </c>
-      <c r="AE4" s="15">
+      <c r="AE4" s="14">
         <f>'[1]Financial Model'!$V$28</f>
         <v>0.1075657234597632</v>
       </c>
-      <c r="AF4" s="15">
+      <c r="AF4" s="14">
         <f>'[1]Financial Model'!$V$29</f>
         <v>6.9837447320891033E-2</v>
       </c>
-      <c r="AG4" s="15">
+      <c r="AG4" s="14">
         <f>'[1]Financial Model'!$V$30</f>
         <v>0.20183486238532111</v>
       </c>
-      <c r="AI4" s="15">
+      <c r="AI4" s="14">
         <f>'[1]Financial Model'!$V$24</f>
         <v>6.633854055210775E-2</v>
       </c>
-      <c r="AJ4" s="15">
+      <c r="AJ4" s="14">
         <f>'[1]Financial Model'!$V$24</f>
         <v>6.633854055210775E-2</v>
       </c>
-      <c r="AK4" s="15">
+      <c r="AK4" s="14">
         <f>'[1]Financial Model'!$U$24</f>
         <v>-2.6747267738223557E-2</v>
       </c>
-      <c r="AL4" s="15">
+      <c r="AL4" s="14">
         <f>'[1]Financial Model'!$T$24</f>
         <v>0.25909722774006405</v>
       </c>
-      <c r="AM4" s="15">
+      <c r="AM4" s="14">
         <f>'[1]Financial Model'!$S$24</f>
         <v>9.3822238221378251E-2</v>
       </c>
-      <c r="AN4" s="15">
+      <c r="AN4" s="14">
         <f>'[1]Financial Model'!$R$24</f>
         <v>0.15066760138121227</v>
       </c>
-      <c r="AO4" s="15">
+      <c r="AO4" s="14">
         <f>'[1]Financial Model'!$Q$24</f>
         <v>0.2464935449630965</v>
       </c>
-      <c r="AP4" s="15">
+      <c r="AP4" s="14">
         <f>'[1]Financial Model'!$P$24</f>
         <v>0.19426026330464774</v>
       </c>
-      <c r="AR4" s="16">
+      <c r="AR4" s="15">
         <f>[1]Main!$C$29</f>
         <v>39484</v>
       </c>
@@ -1323,60 +1358,60 @@
         <f>[2]Main!$C$29</f>
         <v>FY22</v>
       </c>
-      <c r="L8" s="20">
+      <c r="L8" s="19">
         <f>[2]Main!$D$29</f>
         <v>44713</v>
       </c>
-      <c r="Q8" s="19">
+      <c r="Q8" s="18">
         <f>[2]Main!$C$34</f>
         <v>0.64957894736842103</v>
       </c>
-      <c r="R8" s="19">
+      <c r="R8" s="18">
         <f>[2]Main!$C$35</f>
         <v>0.26133031542056079</v>
       </c>
-      <c r="S8" s="19">
+      <c r="S8" s="18">
         <f>[2]Main!$C$36</f>
         <v>0.22496933411214953</v>
       </c>
-      <c r="T8" s="19">
+      <c r="T8" s="18">
         <f>[2]Main!$C$37</f>
         <v>4.6064092664092673</v>
       </c>
-      <c r="U8" s="19">
+      <c r="U8" s="18">
         <f>[2]Main!$C$38</f>
         <v>3.9654826254826259</v>
       </c>
-      <c r="AD8" s="15">
-        <f>'[2]Financial Model'!$X$19</f>
+      <c r="AD8" s="14">
+        <f>'[2]Financial Model'!$Z$19</f>
         <v>0.52694217289719625</v>
       </c>
-      <c r="AE8" s="15">
-        <f>'[2]Financial Model'!$X$20</f>
+      <c r="AE8" s="14">
+        <f>'[2]Financial Model'!$Z$20</f>
         <v>7.878212616822429E-2</v>
       </c>
-      <c r="AF8" s="15">
-        <f>'[2]Financial Model'!$X$21</f>
+      <c r="AF8" s="14">
+        <f>'[2]Financial Model'!$Z$21</f>
         <v>5.6731892523364483E-2</v>
       </c>
-      <c r="AG8" s="15">
-        <f>'[2]Financial Model'!$X$22</f>
+      <c r="AG8" s="14">
+        <f>'[2]Financial Model'!$Z$22</f>
         <v>0.19565217391304351</v>
       </c>
-      <c r="AI8" s="15">
+      <c r="AI8" s="14">
+        <f>'[2]Financial Model'!$Z$16</f>
+        <v>5.9815832237096522E-2</v>
+      </c>
+      <c r="AJ8" s="14">
+        <f>'[2]Financial Model'!$Z$16</f>
+        <v>5.9815832237096522E-2</v>
+      </c>
+      <c r="AK8" s="14">
+        <f>'[2]Financial Model'!$Y$16</f>
+        <v>0.11877759501341889</v>
+      </c>
+      <c r="AL8" s="14">
         <f>'[2]Financial Model'!$X$16</f>
-        <v>5.9815832237096522E-2</v>
-      </c>
-      <c r="AJ8" s="15">
-        <f>'[2]Financial Model'!$X$16</f>
-        <v>5.9815832237096522E-2</v>
-      </c>
-      <c r="AK8" s="15">
-        <f>'[2]Financial Model'!$W$16</f>
-        <v>0.11877759501341889</v>
-      </c>
-      <c r="AL8" s="15">
-        <f>'[2]Financial Model'!$V$16</f>
         <v>1.4491480765852716E-2</v>
       </c>
       <c r="AS8" s="2">

</xml_diff>

<commit_message>
£HFD basic DCF (not finished)
</commit_message>
<xml_diff>
--- a/Overview - Retailers.xlsx
+++ b/Overview - Retailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5C1E81-7346-431F-A004-4FE7CDAF3281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31845B63-C06D-40B9-96CB-27E504E06884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8CE0BD80-0294-417F-B513-C2C882DCE57C}"/>
   </bookViews>
@@ -545,6 +545,9 @@
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
@@ -846,6 +849,9 @@
           <cell r="Z20">
             <v>7.878212616822429E-2</v>
           </cell>
+          <cell r="AL20">
+            <v>0.06</v>
+          </cell>
         </row>
         <row r="21">
           <cell r="Z21">
@@ -855,6 +861,16 @@
         <row r="22">
           <cell r="Z22">
             <v>0.19565217391304351</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="AL24">
+            <v>2.3666166665011588</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="AL26">
+            <v>0.36012452097767755</v>
           </cell>
         </row>
       </sheetData>
@@ -1563,6 +1579,18 @@
         <f>[2]Main!$D$29</f>
         <v>44713</v>
       </c>
+      <c r="M8" s="20">
+        <f>'[2]Financial Model'!$AL$24</f>
+        <v>2.3666166665011588</v>
+      </c>
+      <c r="N8" s="22">
+        <f>'[2]Financial Model'!$AL$26</f>
+        <v>0.36012452097767755</v>
+      </c>
+      <c r="O8" s="22">
+        <f>'[2]Financial Model'!$AL$20</f>
+        <v>0.06</v>
+      </c>
       <c r="Q8" s="18">
         <f>[2]Main!$C$34</f>
         <v>0.64957894736842103</v>

</xml_diff>

<commit_message>
£WRKS 20/21 results data
</commit_message>
<xml_diff>
--- a/Overview - Retailers.xlsx
+++ b/Overview - Retailers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04078E36-5747-44EA-B498-EACE3B259AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E403728-FAD4-4569-A078-7626A529B2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8CE0BD80-0294-417F-B513-C2C882DCE57C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="114">
   <si>
     <t>Ticker</t>
   </si>
@@ -379,6 +379,9 @@
   </si>
   <si>
     <t>Discount Hobbies</t>
+  </si>
+  <si>
+    <t>Stores</t>
   </si>
 </sst>
 </file>
@@ -478,7 +481,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -553,6 +556,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -638,6 +644,11 @@
             <v>2014</v>
           </cell>
         </row>
+        <row r="27">
+          <cell r="C27">
+            <v>1140</v>
+          </cell>
+        </row>
         <row r="29">
           <cell r="C29">
             <v>39484</v>
@@ -755,7 +766,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -823,6 +834,9 @@
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
@@ -1035,6 +1049,16 @@
             <v>2018</v>
           </cell>
         </row>
+        <row r="27">
+          <cell r="C27">
+            <v>526</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29">
+            <v>4044</v>
+          </cell>
+        </row>
         <row r="31">
           <cell r="C31" t="str">
             <v>FY23</v>
@@ -1070,7 +1094,27 @@
         </row>
       </sheetData>
       <sheetData sheetId="1">
+        <row r="16">
+          <cell r="S16">
+            <v>-17.701999999999995</v>
+          </cell>
+          <cell r="T16">
+            <v>-2.2989999999999986</v>
+          </cell>
+          <cell r="U16">
+            <v>13.962999999999985</v>
+          </cell>
+          <cell r="V16">
+            <v>5.2709999999999821</v>
+          </cell>
+        </row>
         <row r="20">
+          <cell r="T20">
+            <v>-0.19712764728361809</v>
+          </cell>
+          <cell r="U20">
+            <v>0.46463360637591311</v>
+          </cell>
           <cell r="V20">
             <v>5.8466538185390826E-2</v>
           </cell>
@@ -1398,13 +1442,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3899F0EA-EAFF-4465-A771-1671EE94CF00}">
-  <dimension ref="B1:AY37"/>
+  <dimension ref="B1:AZ37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P24" sqref="P24"/>
+      <selection pane="bottomRight" activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1427,32 +1471,33 @@
     <col min="34" max="34" width="9.140625" style="1"/>
     <col min="35" max="42" width="9.140625" style="2"/>
     <col min="43" max="43" width="9.140625" style="1"/>
-    <col min="44" max="44" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="45" max="46" width="9.140625" style="2"/>
-    <col min="47" max="47" width="19.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="9.140625" style="1"/>
-    <col min="49" max="49" width="21.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="36.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="52" max="16384" width="9.140625" style="1"/>
+    <col min="44" max="44" width="9.140625" style="15"/>
+    <col min="45" max="45" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="9.140625" style="2"/>
+    <col min="48" max="48" width="19.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.140625" style="1"/>
+    <col min="50" max="50" width="21.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="36.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="53" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:51" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F1" s="28" t="s">
+    <row r="1" spans="2:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F1" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="W1" s="28" t="s">
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="W1" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
       <c r="AC1" s="2"/>
       <c r="AI1" s="14"/>
       <c r="AJ1" s="14"/>
@@ -1462,9 +1507,9 @@
       <c r="AN1" s="14"/>
       <c r="AO1" s="14"/>
       <c r="AP1" s="14"/>
-      <c r="AR1" s="15"/>
-    </row>
-    <row r="2" spans="2:51" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AS1" s="15"/>
+    </row>
+    <row r="2" spans="2:52" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1578,28 +1623,31 @@
         <v>49</v>
       </c>
       <c r="AR2" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS2" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="AS2" s="7" t="s">
+      <c r="AT2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AT2" s="7" t="s">
+      <c r="AU2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AU2" s="7" t="s">
+      <c r="AV2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="AW2" s="7" t="s">
+      <c r="AX2" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AX2" s="7" t="s">
+      <c r="AY2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AY2" s="7" t="s">
+      <c r="AZ2" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
@@ -1745,32 +1793,36 @@
         <v>0.19426026330464774</v>
       </c>
       <c r="AR4" s="15">
+        <f>[1]Main!$C$27</f>
+        <v>1140</v>
+      </c>
+      <c r="AS4" s="15">
         <f>[1]Main!$C$29</f>
         <v>39484</v>
       </c>
-      <c r="AS4" s="2">
+      <c r="AT4" s="2">
         <f>[1]Main!$C$24</f>
         <v>1978</v>
       </c>
-      <c r="AT4" s="2">
+      <c r="AU4" s="2">
         <f>[1]Main!$C$25</f>
         <v>2014</v>
       </c>
-      <c r="AU4" s="2" t="str">
+      <c r="AV4" s="2" t="str">
         <f>[1]Main!$C$23</f>
         <v>Luxembourg/Liverpool</v>
       </c>
-      <c r="AW4" s="2" t="s">
+      <c r="AX4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AX4" s="2" t="s">
+      <c r="AY4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AY4" s="2" t="s">
+      <c r="AZ4" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B8" s="8" t="s">
         <v>57</v>
       </c>
@@ -1803,33 +1855,33 @@
         <f>[2]Main!$C$12</f>
         <v>539.23599999999999</v>
       </c>
-      <c r="AR8" s="2">
+      <c r="AS8" s="2">
         <f>[2]Main!$C$29</f>
         <v>0</v>
       </c>
-      <c r="AS8" s="2">
+      <c r="AT8" s="2">
         <f>[2]Main!$C$24</f>
         <v>1884</v>
       </c>
-      <c r="AT8" s="2">
+      <c r="AU8" s="2">
         <f>[2]Main!$C$25</f>
         <v>2014</v>
       </c>
-      <c r="AU8" s="2" t="str">
+      <c r="AV8" s="2" t="str">
         <f>[2]Main!$C$23</f>
         <v>London, UK</v>
       </c>
-      <c r="AW8" s="2" t="s">
+      <c r="AX8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AX8" s="2" t="s">
+      <c r="AY8" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AY8" s="2" t="s">
+      <c r="AZ8" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
         <v>51</v>
       </c>
@@ -1974,26 +2026,26 @@
         <f>'[3]Financial Model'!$U$16</f>
         <v>7.1953010279001361E-2</v>
       </c>
-      <c r="AS9" s="2">
+      <c r="AT9" s="2">
         <f>[3]Main!$C$24</f>
         <v>1892</v>
       </c>
-      <c r="AT9" s="2">
+      <c r="AU9" s="2">
         <f>[3]Main!$C$25</f>
         <v>2004</v>
       </c>
-      <c r="AU9" s="2" t="str">
+      <c r="AV9" s="2" t="str">
         <f>[3]Main!$C$23</f>
         <v>Redditch, UK</v>
       </c>
-      <c r="AW9" s="2" t="s">
+      <c r="AX9" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AX9" s="2" t="s">
+      <c r="AY9" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
         <v>100</v>
       </c>
@@ -2057,6 +2109,24 @@
         <f>[4]Main!$C$40</f>
         <v>3.0192563081009398</v>
       </c>
+      <c r="W11" s="15">
+        <f>'[4]Financial Model'!$V$16</f>
+        <v>5.2709999999999821</v>
+      </c>
+      <c r="X11" s="15">
+        <f>'[4]Financial Model'!$U$16</f>
+        <v>13.962999999999985</v>
+      </c>
+      <c r="Y11" s="15">
+        <f>'[4]Financial Model'!$T$16</f>
+        <v>-2.2989999999999986</v>
+      </c>
+      <c r="Z11" s="15">
+        <f>'[4]Financial Model'!$S$16</f>
+        <v>-17.701999999999995</v>
+      </c>
+      <c r="AA11" s="15"/>
+      <c r="AB11" s="15"/>
       <c r="AD11" s="14">
         <f>'[4]Financial Model'!$V$23</f>
         <v>0.15672862028832346</v>
@@ -2081,26 +2151,42 @@
         <f>'[4]Financial Model'!$V$20</f>
         <v>5.8466538185390826E-2</v>
       </c>
-      <c r="AS11" s="2">
+      <c r="AK11" s="14">
+        <f>'[4]Financial Model'!$U$20</f>
+        <v>0.46463360637591311</v>
+      </c>
+      <c r="AL11" s="14">
+        <f>'[4]Financial Model'!$T$20</f>
+        <v>-0.19712764728361809</v>
+      </c>
+      <c r="AR11" s="15">
+        <f>[4]Main!$C$27</f>
+        <v>526</v>
+      </c>
+      <c r="AS11" s="15">
+        <f>[4]Main!$C$29</f>
+        <v>4044</v>
+      </c>
+      <c r="AT11" s="2">
         <f>[4]Main!$C$24</f>
         <v>1981</v>
       </c>
-      <c r="AT11" s="2">
+      <c r="AU11" s="2">
         <f>[4]Main!$C$25</f>
         <v>2018</v>
       </c>
-      <c r="AU11" s="2" t="str">
+      <c r="AV11" s="2" t="str">
         <f>[4]Main!$C$23</f>
         <v>Birmingham, UK</v>
       </c>
-      <c r="AW11" s="2" t="s">
+      <c r="AX11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AX11" s="2" t="s">
+      <c r="AY11" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="2:51" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:52" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
       <c r="F16" s="24"/>
@@ -2136,15 +2222,16 @@
       <c r="AN16" s="23"/>
       <c r="AO16" s="23"/>
       <c r="AP16" s="23"/>
-      <c r="AR16" s="23"/>
+      <c r="AR16" s="28"/>
       <c r="AS16" s="23"/>
       <c r="AT16" s="23"/>
       <c r="AU16" s="23"/>
-      <c r="AW16" s="23"/>
+      <c r="AV16" s="23"/>
       <c r="AX16" s="23"/>
       <c r="AY16" s="23"/>
-    </row>
-    <row r="17" spans="2:51" x14ac:dyDescent="0.2">
+      <c r="AZ16" s="23"/>
+    </row>
+    <row r="17" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>55</v>
       </c>
@@ -2154,11 +2241,11 @@
       <c r="E17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AX17" s="2" t="s">
+      <c r="AY17" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>61</v>
       </c>
@@ -2168,11 +2255,11 @@
       <c r="E18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AX18" s="2" t="s">
+      <c r="AY18" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>75</v>
       </c>
@@ -2182,11 +2269,11 @@
       <c r="E19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AX19" s="2" t="s">
+      <c r="AY19" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>59</v>
       </c>
@@ -2196,11 +2283,11 @@
       <c r="E20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AX20" s="2" t="s">
+      <c r="AY20" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>63</v>
       </c>
@@ -2210,14 +2297,14 @@
       <c r="E21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AX21" s="2" t="s">
+      <c r="AY21" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AY21" s="2" t="s">
+      <c r="AZ21" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>65</v>
       </c>
@@ -2227,14 +2314,14 @@
       <c r="E22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AW22" s="2" t="s">
+      <c r="AX22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AX22" s="2" t="s">
+      <c r="AY22" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>67</v>
       </c>
@@ -2244,14 +2331,14 @@
       <c r="E23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AW23" s="2" t="s">
+      <c r="AX23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AX23" s="2" t="s">
+      <c r="AY23" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>95</v>
       </c>
@@ -2266,14 +2353,14 @@
       <c r="M24" s="11"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
-      <c r="AW24" s="2" t="s">
+      <c r="AX24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AX24" s="2" t="s">
+      <c r="AY24" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>98</v>
       </c>
@@ -2288,14 +2375,14 @@
       <c r="M25" s="11"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
-      <c r="AW25" s="2" t="s">
+      <c r="AX25" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AX25" s="2" t="s">
+      <c r="AY25" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>91</v>
       </c>
@@ -2310,14 +2397,14 @@
       <c r="M26" s="11"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
-      <c r="AW26" s="2" t="s">
+      <c r="AX26" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AX26" s="2" t="s">
+      <c r="AY26" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>92</v>
       </c>
@@ -2332,14 +2419,14 @@
       <c r="M27" s="11"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
-      <c r="AW27" s="2" t="s">
+      <c r="AX27" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AX27" s="2" t="s">
+      <c r="AY27" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>103</v>
       </c>
@@ -2354,14 +2441,14 @@
       <c r="M28" s="11"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
-      <c r="AX28" s="2" t="s">
+      <c r="AY28" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="AY28" s="2" t="s">
+      <c r="AZ28" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>110</v>
       </c>
@@ -2377,14 +2464,14 @@
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:52" x14ac:dyDescent="0.2">
       <c r="K30" s="11"/>
       <c r="L30" s="11"/>
       <c r="M30" s="11"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>78</v>
       </c>
@@ -2399,11 +2486,11 @@
       <c r="M31" s="11"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
-      <c r="AX31" s="2" t="s">
+      <c r="AY31" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="2:51" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:52" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>81</v>
       </c>
@@ -2418,11 +2505,11 @@
       <c r="M32" s="11"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
-      <c r="AW32" s="2" t="s">
+      <c r="AX32" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="2:50" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>83</v>
       </c>
@@ -2432,11 +2519,11 @@
       <c r="E33" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AW33" s="2" t="s">
+      <c r="AX33" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="2:50" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>85</v>
       </c>
@@ -2451,11 +2538,11 @@
       <c r="M34" s="11"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
-      <c r="AX34" s="2" t="s">
+      <c r="AY34" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="2:50" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:51" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>87</v>
       </c>
@@ -2470,18 +2557,18 @@
       <c r="M35" s="11"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
-      <c r="AX35" s="2" t="s">
+      <c r="AY35" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="2:50" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:51" x14ac:dyDescent="0.2">
       <c r="K36" s="11"/>
       <c r="L36" s="11"/>
       <c r="M36" s="11"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
     </row>
-    <row r="37" spans="2:50" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:51" x14ac:dyDescent="0.2">
       <c r="K37" s="11"/>
       <c r="L37" s="11"/>
       <c r="M37" s="11"/>

</xml_diff>

<commit_message>
£WRKS start historical interims
</commit_message>
<xml_diff>
--- a/Overview - Retailers.xlsx
+++ b/Overview - Retailers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A424C03-96FF-473A-BCA6-71BA4D490411}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAFCB95-6F47-415F-AF01-620FD9657E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8CE0BD80-0294-417F-B513-C2C882DCE57C}"/>
   </bookViews>
@@ -26,12 +26,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="116">
   <si>
     <t>Ticker</t>
   </si>
@@ -373,6 +382,12 @@
   </si>
   <si>
     <t>Stores</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>The Works &amp; TheWorks.co.uk</t>
   </si>
 </sst>
 </file>
@@ -583,7 +598,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -761,7 +776,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -820,7 +835,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -983,8 +998,11 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
@@ -1433,10 +1451,10 @@
   <dimension ref="B1:AZ37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AB3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AO3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AN12" sqref="AN12"/>
+      <selection pane="bottomRight" activeCell="AZ12" sqref="AZ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2155,6 +2173,12 @@
         <f>+'[4]Financial Model'!$R$20</f>
         <v>0.1320614263404476</v>
       </c>
+      <c r="AO11" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP11" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="AR11" s="15">
         <f>[4]Main!$C$27</f>
         <v>526</v>
@@ -2180,6 +2204,9 @@
       </c>
       <c r="AY11" s="2" t="s">
         <v>112</v>
+      </c>
+      <c r="AZ11" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="2:52" s="22" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>